<commit_message>
#processing the latest pH runs on the first day of processing the backlog of samples for pH. most values looked pretty good. P-0036B-1 had a 0.05 pH unit difference and may need to be reran a third time on the next processing round
</commit_message>
<xml_diff>
--- a/check sample work/pH QAQC/processed pH data/buoy_samples_metadata_2019.xlsx
+++ b/check sample work/pH QAQC/processed pH data/buoy_samples_metadata_2019.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\915712257\Box Sync\Nielsen Lab\RTC CeNCOOS\Seawater Chemistry\Data\pH data\processed\buoy check samples\2019 check samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2020-season-summary\check sample work\pH QAQC\processed pH data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23711958-A3BB-4D70-9814-1C0A4DDF8A26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12036" windowHeight="2136"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="buoy_samples_metadata_2019" sheetId="1" r:id="rId1"/>
     <sheet name="readme" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1097,7 +1097,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -1105,24 +1105,24 @@
       <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="86.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="86.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43532</v>
       </c>
@@ -1206,7 +1206,7 @@
       <c r="N2" s="6"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>43532</v>
       </c>
@@ -1243,7 +1243,7 @@
       <c r="N3" s="6"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43532</v>
       </c>
@@ -1280,7 +1280,7 @@
       <c r="N4" s="6"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43532</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="N5" s="6"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43532</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="N6" s="6"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>43532</v>
       </c>
@@ -1391,7 +1391,7 @@
       <c r="N7" s="6"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43532</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>43535</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>12.1997</v>
       </c>
       <c r="F9" s="9">
-        <f t="shared" ref="F3:F9" si="0">MEDIAN(G9:I9)</f>
+        <f t="shared" ref="F9" si="0">MEDIAN(G9:I9)</f>
         <v>7.9831010909762803</v>
       </c>
       <c r="G9" s="2">
@@ -1471,7 +1471,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>43566</v>
       </c>
@@ -1509,7 +1509,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43585</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43585</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>43585</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43585</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>43586</v>
       </c>
@@ -1684,7 +1684,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>43586</v>
       </c>
@@ -1722,7 +1722,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>43606</v>
       </c>
@@ -1760,7 +1760,7 @@
       <c r="N17" s="2"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43606</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>43606</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43606</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>43641</v>
       </c>
@@ -1927,7 +1927,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>43641</v>
       </c>
@@ -1965,7 +1965,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>43656</v>
       </c>
@@ -2002,7 +2002,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>43656</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>43677</v>
       </c>
@@ -2076,7 +2076,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="3"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>43692</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="N26" s="2"/>
       <c r="O26" s="3"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>43692</v>
       </c>
@@ -2150,7 +2150,7 @@
       <c r="N27" s="2"/>
       <c r="O27" s="3"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>43725</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="N28" s="2"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>43747</v>
       </c>
@@ -2224,7 +2224,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="3"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>43747</v>
       </c>
@@ -2261,7 +2261,7 @@
       <c r="N30" s="2"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>43762</v>
       </c>
@@ -2298,7 +2298,7 @@
       <c r="N31" s="2"/>
       <c r="O31" s="3"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>43775</v>
       </c>
@@ -2331,7 +2331,7 @@
       <c r="N32" s="6"/>
       <c r="O32" s="3"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>43775</v>
       </c>
@@ -2364,7 +2364,7 @@
       <c r="N33" s="6"/>
       <c r="O33" s="3"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>43775</v>
       </c>
@@ -2397,7 +2397,7 @@
       <c r="N34" s="6"/>
       <c r="O34" s="3"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>43775</v>
       </c>
@@ -2427,7 +2427,7 @@
       <c r="N35" s="6"/>
       <c r="O35" s="3"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>43775</v>
       </c>
@@ -2466,20 +2466,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>48</v>
       </c>

</xml_diff>